<commit_message>
Added new Chromedriver Structure
Also added .gitignore now to remove iml conflicts in the future.
</commit_message>
<xml_diff>
--- a/exampleProject/com.runner.report.xlsx
+++ b/exampleProject/com.runner.report.xlsx
@@ -39,13 +39,13 @@
     <t>Passed Tests</t>
   </si>
   <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>Failed Tests</t>
+  </si>
+  <si>
     <t>0%</t>
-  </si>
-  <si>
-    <t>Failed Tests</t>
-  </si>
-  <si>
-    <t>100%</t>
   </si>
   <si>
     <t>Tests Not Run</t>
@@ -294,7 +294,7 @@
         <f>SUM(E17:E100)</f>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -305,7 +305,7 @@
         <f>SUM(F17:F100)</f>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -336,10 +336,10 @@
         <v>19</v>
       </c>
       <c r="C14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1.0</v>
       </c>
       <c r="E14" t="n">
         <v>0.0</v>
@@ -363,7 +363,7 @@
   <cols>
     <col min="1" max="1" width="51.375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="57.01171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="6.87109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="6.94140625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.9453125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="7.91796875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="43.39453125" customWidth="true" bestFit="true"/>
@@ -429,7 +429,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>

</xml_diff>